<commit_message>
Pacote de Atualização 1.0
</commit_message>
<xml_diff>
--- a/desafioFinanceiro/DesafioPoupança2reais.xlsx
+++ b/desafioFinanceiro/DesafioPoupança2reais.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Semana</t>
   </si>
@@ -627,23 +627,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -994,7 +994,7 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1014,15 +1014,15 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="56" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="39" t="s">
@@ -1159,10 +1159,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="E8" s="53"/>
+      <c r="E8" s="53" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
+      <c r="G8" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="58"/>
@@ -2041,29 +2047,29 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
-      <c r="B57" s="60" t="s">
+      <c r="B57" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
-      <c r="H57" s="60"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
     </row>
     <row r="58" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="41">
         <v>1</v>
       </c>
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="61"/>
-      <c r="H58" s="61"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
     </row>
     <row r="59" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="42"/>
@@ -2079,15 +2085,15 @@
       <c r="A60" s="41">
         <v>2</v>
       </c>
-      <c r="B60" s="61" t="s">
+      <c r="B60" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
     </row>
     <row r="61" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="45"/>
@@ -2103,15 +2109,15 @@
       <c r="A62" s="41">
         <v>3</v>
       </c>
-      <c r="B62" s="61" t="s">
+      <c r="B62" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
     </row>
     <row r="63" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="48"/>
@@ -2285,11 +2291,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="A54:A55"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
@@ -2305,6 +2306,11 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="A54:A55"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Pacote de Atualizações 1.1
</commit_message>
<xml_diff>
--- a/desafioFinanceiro/DesafioPoupança2reais.xlsx
+++ b/desafioFinanceiro/DesafioPoupança2reais.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Semana</t>
   </si>
@@ -994,7 +994,7 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1183,9 +1183,13 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="E9" s="53"/>
+      <c r="E9" s="53" t="s">
+        <v>24</v>
+      </c>
       <c r="F9" s="53"/>
-      <c r="G9" s="54"/>
+      <c r="G9" s="54" t="s">
+        <v>24</v>
+      </c>
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>